<commit_message>
new season update commit
</commit_message>
<xml_diff>
--- a/execution_log/execution_log.xlsx
+++ b/execution_log/execution_log.xlsx
@@ -344,7 +344,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D369"/>
+  <dimension ref="A1:D371"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6249,7 +6249,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1">
-        <v>45804.53088094995</v>
+        <v>45804.53088094907</v>
       </c>
       <c r="B369">
         <v>5</v>
@@ -6258,6 +6258,38 @@
         <v>368</v>
       </c>
       <c r="D369" t="inlineStr">
+        <is>
+          <t>data model updated</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1">
+        <v>45887.45433633102</v>
+      </c>
+      <c r="B370">
+        <v>15</v>
+      </c>
+      <c r="C370">
+        <v>369</v>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>data model updated</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1">
+        <v>45887.47151704012</v>
+      </c>
+      <c r="B371">
+        <v>9</v>
+      </c>
+      <c r="C371">
+        <v>370</v>
+      </c>
+      <c r="D371" t="inlineStr">
         <is>
           <t>data model updated</t>
         </is>

</xml_diff>